<commit_message>
add zutnlp_text Framework and weekly reports
</commit_message>
<xml_diff>
--- a/zutnlp-master/zutnlp-text/doc/log/卢思童.xlsx
+++ b/zutnlp-master/zutnlp-text/doc/log/卢思童.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14130" windowHeight="7950"/>
+    <workbookView windowWidth="20385" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32">
   <si>
     <t>日志报告</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>仿造老师的模板搭建IDEA</t>
+  </si>
+  <si>
+    <t>2018.07.23</t>
+  </si>
+  <si>
+    <t>仿造模板搭建IDEA</t>
+  </si>
+  <si>
+    <t>导入数据库</t>
   </si>
 </sst>
 </file>
@@ -162,21 +171,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,12 +200,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -229,14 +254,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,7 +269,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,25 +307,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,187 +323,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,6 +541,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -547,11 +567,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -580,28 +606,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -613,10 +622,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -625,133 +634,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1096,10 +1105,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:I17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1322,45 +1331,95 @@
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="4"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="6"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="6"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="36">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -1372,6 +1431,7 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="B3:C4"/>
     <mergeCell ref="D3:E4"/>
     <mergeCell ref="F3:I4"/>
@@ -1393,6 +1453,9 @@
     <mergeCell ref="B15:C17"/>
     <mergeCell ref="D15:E17"/>
     <mergeCell ref="F15:I17"/>
+    <mergeCell ref="B18:C21"/>
+    <mergeCell ref="D18:E21"/>
+    <mergeCell ref="F18:I21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>